<commit_message>
Consolidated colors, reordered inputs on acoustic setup, Fixed positions
</commit_message>
<xml_diff>
--- a/Assets/BandColorConvention.xlsx
+++ b/Assets/BandColorConvention.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEBB256-C339-430C-BF86-766962F5567F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D7839E-7813-4838-BBBB-A6E49DDFB8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -98,31 +98,31 @@
     <t>Upstage Center</t>
   </si>
   <si>
-    <t>Stage Right</t>
-  </si>
-  <si>
-    <t>Stage Left</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>Center Stage Right</t>
-  </si>
-  <si>
-    <t>CSR</t>
-  </si>
-  <si>
-    <t>CSL</t>
-  </si>
-  <si>
-    <t>Center Stage Left</t>
-  </si>
-  <si>
-    <t>Drum</t>
+    <t>DCR</t>
+  </si>
+  <si>
+    <t>DCL</t>
+  </si>
+  <si>
+    <t>Downstage Center Right</t>
+  </si>
+  <si>
+    <t>Downstage Center Left</t>
+  </si>
+  <si>
+    <t>Downstage Right</t>
+  </si>
+  <si>
+    <t>DSR</t>
+  </si>
+  <si>
+    <t>DSL</t>
+  </si>
+  <si>
+    <t>Downstage Left</t>
+  </si>
+  <si>
+    <t>USC</t>
   </si>
 </sst>
 </file>
@@ -555,12 +555,14 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -607,10 +609,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>15</v>
@@ -624,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -641,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -658,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>14</v>

</xml_diff>